<commit_message>
updating the assignment guideline downloads; adding a GenAI policy section to the frontmatter
</commit_message>
<xml_diff>
--- a/assets/assignments/a1_guidelines.xlsx
+++ b/assets/assignments/a1_guidelines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\teaching\utrecht\tcsm\git\tcsm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\teaching\utrecht\isem\git\isem\assets\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE1F3F6-BB4E-495B-AA26-D51B882214B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C1EB72-2183-4115-8882-9599D76441C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20760" xr2:uid="{9D52BE51-53AF-6049-ADAE-4D3E218C8A57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21240" windowHeight="15270" xr2:uid="{9D52BE51-53AF-6049-ADAE-4D3E218C8A57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Gross differences from the required format (e.g., wrong file type, missing sections, submitting multiple files, missing title page or information thereon).</t>
-  </si>
-  <si>
     <t>Results are discussed clearly, and the RQ is clearly answered through this discussion; Strengths and limitations of the analysis are considered.</t>
   </si>
   <si>
@@ -89,27 +86,15 @@
     <t>1. Data description</t>
   </si>
   <si>
-    <t>TCSM Assignment 1: Path Analysis</t>
-  </si>
-  <si>
-    <t>Missing or malformed research question; Insufficient model (e.g., fewer than three variables); Missing or innacurate path diagram; Theoretical model is not described well enough to interpret the results; Theoretical model does not match the RQ.</t>
-  </si>
-  <si>
     <t>All (and only) relevant results are reported and interpreted; Extra attention is applied to formatting tables and figures to optimize clarity; The selection of reported results shows a clear understanding of what information is important.</t>
   </si>
   <si>
-    <t>Results not interpreted or interpreted incorrectly; Applicable measures of explained variance are not included; Importasnt results are omitted; Assumptions are not checked or checked/evaluated incorrectly; Results are included by copying/embedding R output.</t>
-  </si>
-  <si>
     <t>Results are reported in a sensible style and interpreted correctly; Appropriate measures of explained variance are included and discussed; Assumptions are discussed and interpreted; Results are included as correctly typeset in-text statistics or as well-formatted tables or figures.</t>
   </si>
   <si>
     <t>4. Reporting and interpreting results</t>
   </si>
   <si>
-    <t>5. Discussion of results</t>
-  </si>
-  <si>
     <t>Very clear and succinct description that shows good understanding; Extra effort applied to making the data description efficient and effective (e.g., through novel tables or figures); Extra effort applied to processing and cleaning the data.</t>
   </si>
   <si>
@@ -120,6 +105,21 @@
   </si>
   <si>
     <t>The model defined by the analysis script and lavaan syntax snippets correctly answers the research question and matches the reported results; The relevant syntax is provided with the report, and very little extraneous code is included.</t>
+  </si>
+  <si>
+    <t>ISEM Assignment 1: Path Analysis</t>
+  </si>
+  <si>
+    <t>5. Discussion of findings</t>
+  </si>
+  <si>
+    <t>Missing or malformed research question; Insufficient model (e.g., fewer than three variables); Missing or inaccurate path diagram; Theoretical model is not described well enough to interpret the results; Theoretical model does not match the RQ.</t>
+  </si>
+  <si>
+    <t>Results not interpreted or interpreted incorrectly; Applicable measures of explained variance are not included; Important results are omitted; Assumptions are not checked or checked/evaluated incorrectly; Results are included by copying/embedding R output.</t>
+  </si>
+  <si>
+    <t>Gross differences from the required format (e.g., wrong file type, missing sections, submitting redundant files, missing author information).</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -600,7 +600,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -618,92 +618,92 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" s="4" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" s="4" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -715,7 +715,7 @@
     </row>
     <row r="14" spans="1:3" s="4" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -740,9 +740,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -860,25 +863,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4054948-5070-499A-8F80-35FDF67FC4C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{222BBD21-8C3D-4056-8F9E-712DCC33AD59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -900,9 +893,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{222BBD21-8C3D-4056-8F9E-712DCC33AD59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4054948-5070-499A-8F80-35FDF67FC4C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>